<commit_message>
Test scrape done, getHouse fixed
</commit_message>
<xml_diff>
--- a/Scraper/12C Usernames.xlsx
+++ b/Scraper/12C Usernames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bejoy\Desktop\Jayadeep\Code\JavaScript\votingsystem\Scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA33830-D10B-4EE3-AFA7-63FE9C3ABCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3FFFB7-71DF-40A3-9D77-4D778197332D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3519391F-A44B-49F3-A475-500EFD9B6D22}"/>
   </bookViews>
@@ -607,8 +607,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="C2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>